<commit_message>
spreadsheet: add convenience methods
- add a Cell method to the sheet that gets/creates a cell
- chance Row.Cell to not require the row number
- rename EnsureRow to Row
- add examples/tests
</commit_message>
<xml_diff>
--- a/_examples/spreadsheet/named-cells/named-cells.xlsx
+++ b/_examples/spreadsheet/named-cells/named-cells.xlsx
@@ -8,7 +8,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="9" uniqueCount="9">
+<x:sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:sh="http://schemas.openxmlformats.org/officeDocument/2006/sharedTypes" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:xml="http://www.w3.org/XML/1998/namespace" count="13" uniqueCount="13">
   <x:si>
     <x:t>row 0</x:t>
   </x:si>
@@ -35,6 +35,18 @@
   </x:si>
   <x:si>
     <x:t>Cell E26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cell F26</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cell H1</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cell H2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Cell H3</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -87,6 +99,9 @@
       <x:c t="s">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="H1" t="s">
+        <x:v>10</x:v>
+      </x:c>
     </x:row>
     <x:row r="2">
       <x:c t="s">
@@ -98,6 +113,9 @@
       <x:c t="s">
         <x:v>1</x:v>
       </x:c>
+      <x:c r="H2" t="s">
+        <x:v>11</x:v>
+      </x:c>
     </x:row>
     <x:row r="3">
       <x:c t="s">
@@ -108,6 +126,9 @@
       </x:c>
       <x:c t="s">
         <x:v>1</x:v>
+      </x:c>
+      <x:c r="H3" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
     <x:row r="4">
@@ -139,6 +160,9 @@
       <x:c r="E26" t="s">
         <x:v>8</x:v>
       </x:c>
+      <x:c r="F26" t="s">
+        <x:v>9</x:v>
+      </x:c>
     </x:row>
   </x:sheetData>
 </x:worksheet>

</xml_diff>